<commit_message>
export and import worker and contractor
</commit_message>
<xml_diff>
--- a/Presentation/Visitor.API/FormatFiles/Template_Visitor.xlsx
+++ b/Presentation/Visitor.API/FormatFiles/Template_Visitor.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
   <si>
     <t>VisitorName</t>
   </si>
@@ -198,19 +198,16 @@
     <t>SINGLE ENTRY</t>
   </si>
   <si>
-    <t>19-08-2025</t>
-  </si>
-  <si>
     <t>987654321</t>
   </si>
   <si>
     <t>MULTIPLE ENTRY</t>
   </si>
   <si>
-    <t>21-08-2025</t>
-  </si>
-  <si>
     <t>987654322</t>
+  </si>
+  <si>
+    <t>28/08/2025</t>
   </si>
 </sst>
 </file>
@@ -285,7 +282,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -304,6 +301,9 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -719,14 +719,14 @@
       <c r="A2" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>22</v>
@@ -797,16 +797,16 @@
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>64</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
issue and new field added
</commit_message>
<xml_diff>
--- a/Presentation/Visitor.API/FormatFiles/Template_Visitor.xlsx
+++ b/Presentation/Visitor.API/FormatFiles/Template_Visitor.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="86">
   <si>
     <t>VisitorName</t>
   </si>
@@ -208,6 +208,72 @@
   </si>
   <si>
     <t>28/08/2025</t>
+  </si>
+  <si>
+    <t>IsCrew</t>
+  </si>
+  <si>
+    <t>Nationality</t>
+  </si>
+  <si>
+    <t>IsPassport</t>
+  </si>
+  <si>
+    <t>PassportNo</t>
+  </si>
+  <si>
+    <t>PlaceOfIssue</t>
+  </si>
+  <si>
+    <t>PassportIssueDate</t>
+  </si>
+  <si>
+    <t>PassportValidTill</t>
+  </si>
+  <si>
+    <t>Vessel</t>
+  </si>
+  <si>
+    <t>IsForeigner</t>
+  </si>
+  <si>
+    <t>IsVisa</t>
+  </si>
+  <si>
+    <t>VisaNo</t>
+  </si>
+  <si>
+    <t>VisaValidFrom</t>
+  </si>
+  <si>
+    <t>VisaValidTill</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>P101</t>
+  </si>
+  <si>
+    <t>P102</t>
+  </si>
+  <si>
+    <t>28/08/2026</t>
+  </si>
+  <si>
+    <t>28/08/2027</t>
+  </si>
+  <si>
+    <t>28/09/2025</t>
+  </si>
+  <si>
+    <t>VESSEL 1</t>
+  </si>
+  <si>
+    <t>V101</t>
+  </si>
+  <si>
+    <t>28/12/2025</t>
   </si>
 </sst>
 </file>
@@ -282,7 +348,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -302,6 +368,11 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -607,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AM3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AM1" sqref="AM1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -633,9 +704,19 @@
     <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.140625" style="10"/>
+    <col min="28" max="28" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16" style="12" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11" style="12" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14" style="12" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:39">
       <c r="A1" s="4" t="s">
         <v>55</v>
       </c>
@@ -714,8 +795,47 @@
       <c r="Z1" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="AA1" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF1" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG1" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI1" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL1" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM1" s="11" t="s">
+        <v>76</v>
+      </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:39">
       <c r="A2" s="8" t="s">
         <v>59</v>
       </c>
@@ -794,8 +914,38 @@
       <c r="Z2" s="7" t="s">
         <v>40</v>
       </c>
+      <c r="AA2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD2" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF2" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG2" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ2" s="12" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:39">
       <c r="A3" s="8" t="s">
         <v>61</v>
       </c>
@@ -873,6 +1023,45 @@
       </c>
       <c r="Z3" s="7" t="s">
         <v>54</v>
+      </c>
+      <c r="AA3" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB3" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD3" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE3" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF3" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG3" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL3" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM3" s="10" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -881,6 +1070,7 @@
     <hyperlink ref="F3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>